<commit_message>
Changed plot title styling and updated example xlsx
</commit_message>
<xml_diff>
--- a/examples/plotibcs_plot_ibcs_waterfall.xlsx
+++ b/examples/plotibcs_plot_ibcs_waterfall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/62a07d598bdbd2d4/Documents/Development Projects/R/plotibcs/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="8_{33CD71A4-6A61-4501-BF8A-94ED4BC140CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CB9E771-14E8-468F-AA75-645538B29914}"/>
+  <xr:revisionPtr revIDLastSave="160" documentId="8_{33CD71A4-6A61-4501-BF8A-94ED4BC140CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A91E55CB-27CB-4A2C-B832-7EED98E0A094}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -328,16 +328,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>249917</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>254214</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>436037</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>95464</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>228026</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>168703</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>58327</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>97540</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -365,7 +365,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8827892" y="254214"/>
+          <a:off x="436037" y="1628223"/>
           <a:ext cx="6437592" cy="6505351"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -762,7 +762,7 @@
     <we:property name="pyworkerConfig" value="&quot;{\&quot;pyodideVersion\&quot;:\&quot;0.26.4\&quot;,\&quot;pyodidePackages\&quot;:[\&quot;numpy\&quot;,\&quot;pandas\&quot;,\&quot;matplotlib\&quot;,\&quot;statsmodels\&quot;,\&quot;scikit-learn\&quot;],\&quot;pyscriptApps\&quot;:[],\&quot;micropipPackages\&quot;:[\&quot;seaborn==0.13.2\&quot;],\&quot;initCode\&quot;:\&quot;# Add imports\\nimport math\\nimport numpy as np\\nimport pandas as pd\\nfrom sklearn.ensemble import IsolationForest\\n\\n# Define UDF\\n@UDF(name='AUDIT.LEDGER', nested=False)\\ndef detect_anomalies(data: UDF.Range) -&gt; UDF.Range:\\n    df = to_df(data)\\n    df_model = df.copy()\\n\\n    # Ensure correct types\\n    df_model['ACCOUNT'] = df_model['ACCOUNT'].astype(str)\\n    df_model['SOURCE'] = df_model['SOURCE'].astype(str)\\n\\n    # Add engineered features\\n    df_model['ABS_AMOUNT'] = df_model['AMOUNT'].abs()\\n    df_model['Z_AMT_BY_ACCOUNT'] = (\\n        df_model.groupby('ACCOUNT')['AMOUNT']\\n        .transform(lambda x: (x - x.mean()) \/ (x.std(ddof=0) + 1e-6))\\n    )\\n\\n    # Encode categorical\\n    df_encoded = pd.get_dummies(df_model[['ACCOUNT', 'SOURCE']])\\n    X = pd.concat([df_model[['AMOUNT', 'ABS_AMOUNT', 'Z_AMT_BY_ACCOUNT']], df_encoded], axis=1)\\n\\n    # Fit model with higher sensitivity\\n    clf = IsolationForest(contamination=0.1, random_state=42)\\n    df_model['ML_ANOMALY'] = clf.fit_predict(X).astype(int)\\n    df_model['ML_ANOMALY'] = df_model['ML_ANOMALY'].map({1: 0, -1: 1})\\n\\n    return df_model\\n\\n\\n# Pre-built utility functions\\ndef to_df(data) -&gt; pd.DataFrame:\\n    \\\&quot;\\\&quot;\\\&quot;\\n    Converts a REF (i.e. list of lists) into a pandas DataFrame\\n    Assumes that the first row contains column headers\\n\\n    Usage: df = to_df(REF(\\\&quot;F15:H22\\\&quot;))\\n    \\\&quot;\\\&quot;\\\&quot;\\n    if isinstance(data, pd.DataFrame):\\n        return data\\n    if hasattr(data, '__len__') and len(data) &gt; 0 and is_listlike(data[0]):\\n        return pd.DataFrame(data[1:], columns=data[0])\\n    raise TypeError('Expected list of lists')\\n\\ndef to_array(data) -&gt; np.ndarray:\\n    \\\&quot;\\\&quot;\\\&quot;\\n    Converts a REF (i.e. list of lists) into a 2-dimensional numpy array\\n\\n    Usage: arr = to_array(REF(\\\&quot;B3:C44\\\&quot;))\\n    \\\&quot;\\\&quot;\\\&quot;\\n    if isinstance(data, np.ndarray):\\n        return data\\n    return np.array(data)\\n\\ndef to_list(data) -&gt; list:\\n    \\\&quot;\\\&quot;\\\&quot;\\n    Converts a REF (i.e. list of lists) into a 1-d list.\\n    Handles wide (1xn) or tall (nx1) data.\\n\\n    Usage: x = to_list(REF(\\\&quot;G1:G55\\\&quot;))\\n    \\\&quot;\\\&quot;\\\&quot;\\n    if not is_listlike(data): # data is scalar\\n        return [data]\\n    if len(data) == 0 or not is_listlike(data[0]): # already a 1-d list\\n        return list(data)\\n    if len(data) == 1: # data is wide\\n        return list(data[0])\\n    elif len(data[0]) == 1: #data is tall\\n        return [x[0] for x in data]\\n    else:\\n        raise TypeError(f\\\&quot;data must be 1xn or nx1, not {len(data)}x{len(data[0])}\\\&quot;)\\n\\ndef is_listlike(x) -&gt; bool:\\n    return hasattr(x, '__len__') and type(x) not in {str, bytes}\\n\\n\&quot;}&quot;"/>
     <we:property name="registeredUDFs" value="&quot;[[\&quot;AUDIT.LEDGER\&quot;,false,\&quot;detect_anomalies\&quot;,{\&quot;parameters\&quot;:[{\&quot;dimensionality\&quot;:\&quot;matrix\&quot;,\&quot;description\&quot;:\&quot;type Range\&quot;,\&quot;name\&quot;:\&quot;data\&quot;}],\&quot;result\&quot;:{\&quot;dimensionality\&quot;:\&quot;matrix\&quot;},\&quot;options\&quot;:{\&quot;requiresAddress\&quot;:true,\&quot;requiresParameterAddresses\&quot;:true}}]]&quot;"/>
     <we:property name="AnacondaCodeActiveInterpreter" value="&quot;r&quot;"/>
-    <we:property name="rworkerConfig" value="&quot;{\&quot;webrVersion\&quot;:\&quot;0.4.2\&quot;,\&quot;webrPackages\&quot;:[\&quot;jsonlite\&quot;,\&quot;sloop\&quot;,\&quot;tidyverse\&quot;,\&quot;patchwork\&quot;],\&quot;initCode\&quot;:\&quot;## Add imports\\nlibrary(tidyverse)\\nlibrary(patchwork)\\n\\n## Configuration\\noptions(warnPartialMatchDollar = TRUE)\\n\\n## Define functions\\nplot_ibcs_waterfall &lt;- function(\\n  df_raw,\\n  title = \\\&quot;Waterfall Chart\\\&quot;,\\n  value_col = \\\&quot;Value\\\&quot;,\\n  label_col = \\\&quot;Line.Item\\\&quot;\\n) {\\n\\n  # Rename user-specified columns to fixed internal names\\n  df_raw &lt;- df_raw %&gt;%\\n    rename(\\n      Value = all_of(value_col),\\n      `Line.Item` = all_of(label_col)\\n    )\\n\\n  cols &lt;- c(\\\&quot;position\\\&quot;, \\\&quot;type\\\&quot;, \\\&quot;bold\\\&quot;, \\\&quot;subtotal_group\\\&quot;, \\\&quot;Line.Item\\\&quot;, \\\&quot;Value\\\&quot;)\\n  df_raw &lt;- df_raw %&gt;% select(all_of(cols))\\n\\n  # Flag the rows that will be for plotting bars\\n  df &lt;- df_raw %&gt;% mutate(is_plot_row = type != \\\&quot;divider\\\&quot;)\\n\\n  # Assign vertical positions only to non-divider rows\\n  df$x[df$type != \\\&quot;divider\\\&quot;] &lt;- seq_len(sum(df$type != \\\&quot;divider\\\&quot;))\\n\\n  # Compute start\/end for all types\\n  anchor &lt;- 0\\n  for (i in seq_len(nrow(df))) {\\n    row_type &lt;- df$type[i]\\n\\n    if (row_type == \\\&quot;bar\\\&quot;) {\\n      df$start[i] &lt;- anchor\\n      df$end[i] &lt;- anchor + df$Value[i]\\n      anchor &lt;- df$end[i]\\n\\n    } else if (row_type == \\\&quot;subtotal\\\&quot;) {\\n      group_id &lt;- df$subtotal_group[i]\\n      bar_rows &lt;- which(df$subtotal_group == group_id &amp; df$type == \\\&quot;bar\\\&quot;)\\n      if (length(bar_rows) &gt; 0) {\\n        subtotal_value &lt;- sum(df$Value[bar_rows], na.rm = TRUE)\\n        df$Value[i] &lt;- subtotal_value\\n        group_start &lt;- df$start[bar_rows[1]]\\n        df$start[i] &lt;- group_start\\n        df$end[i] &lt;- group_start + subtotal_value\\n        anchor &lt;- df$end[i]\\n      }\\n\\n    } else if (row_type == \\\&quot;result\\\&quot;) {\\n      df$start[i] &lt;- 0\\n      df$end[i] &lt;- anchor\\n      df$Value[i] &lt;- anchor\\n      anchor &lt;- df$end[i]\\n    }\\n  }\\n\\n  # calculate the coordinates for non-subtotal and non-result connecting lines\\n  df_lines &lt;- df %&gt;%\\n    filter(type != \\\&quot;divider\\\&quot;) %&gt;%\\n    arrange(x) %&gt;%\\n    mutate(\\n      x_next = lead(x),\\n      xend = lead(start)\\n    ) %&gt;%\\n    filter(!is.na(x_next)) %&gt;%\\n    transmute(\\n      y = x - 0.3, # from the vertical top of the current bar\\n      yend = x_next + 0.3, # to the vertical bottom of the next bar\\n      x = xend,\\n      xend\\n    )\\n\\n  # Assign fill colors to drawn bars\\n  # Positive bars are gray with 70% transparency\\n  # Negative bars are gray with 30% transparency\\n  df &lt;- df %&gt;%\\n    mutate(\\n      fill = case_when(\\n        type == \\\&quot;divider\\\&quot; ~ NA_character_,\\n        Value &gt;= 0 ~ \\\&quot;gray70\\\&quot;,\\n        TRUE ~ \\\&quot;gray30\\\&quot;\\n      )\\n    )\\n\\n  # Format the bar labels\\n  # Currently zero decimal places\\n  # Negative bars have their labels to the left of the bar\\n  # Positive bars have their labels to the right of the bar\\n  # Negative bars don't use the minus symbol\\n  df_labels &lt;- df %&gt;%\\n    filter(type != \\\&quot;divider\\\&quot;) %&gt;%\\n    mutate(\\n      label = format(round(abs(Value), 0), nsmall = 0),\\n      label_x = if_else(Value &gt;= 0, end + 5, end - 5),\\n      hjust = if_else(Value &gt;= 0, 0, 1)\\n    )\\n\\n  # this will be used to extend the x-axis to allow space for bar labels\\n  # x_max &lt;- max(df_labels$label_x, na.rm = TRUE) + 100  # 10 is padding\\n\\n  # divider_ys is a numeric vector of vertical positions\\n  # at which horizontal lines will be drawn to separate\\n  # bars from one another at the user's discretion\\n  divider_ys &lt;- df %&gt;%\\n    mutate(idx = row_number()) %&gt;%\\n    filter(type == \\\&quot;divider\\\&quot;) %&gt;%\\n    mutate(\\n      prev_x = df$x[idx - 1],\\n      next_x = df$x[idx + 1],\\n      y = (prev_x + next_x) \/ 2\\n    ) %&gt;%\\n    pull(y) # extracts this tibble column to a vector\\n\\n  df_subtotals &lt;- df %&gt;% filter(type == \\\&quot;subtotal\\\&quot;)\\n\\n  # Apply a function over a list of integers from 1 to count of sub total rows\\n  df_sub_connectors &lt;- bind_rows(lapply(seq_len(nrow(df_subtotals)), function(i) {\\n    # Get the current row\\n    subtotal_row &lt;- df_subtotals[i, ]\\n    # Get the current group id\\n    group_id &lt;- subtotal_row$subtotal_group\\n    # Get the bar rows from df whose group id matches the current subtotal row\\n    bar_rows &lt;- df %&gt;% filter(type == \\\&quot;bar\\\&quot;, subtotal_group == group_id)\\n\\n    # If there are no such bars, then this subtotal is invalid (user incorrectly defined)\\n    if (nrow(bar_rows) &lt; 1) return(NULL)\\n\\n    # There are two lines which visually connect a subtotal with its components:\\n    # 1) A line from the bottom (i.e. left) of the first bar in the group\\n    # to the bottom (i.e. left) of the sub-total bar\\n    # 2) A line from the top (i.e. right) of the last bar in the group\\n    # to the top (i.e. right) of the sub-total bar\\n    first_bar &lt;- bar_rows[1, ]\\n    last_bar &lt;- bar_rows[nrow(bar_rows), ]\\n\\n    # Each sub-total produces two rows representing the lines connecting the \\n    # bars with their associated sub-total bar\\n    tibble(\\n      x = c(first_bar$start, last_bar$end),\\n      xend = c(first_bar$start, last_bar$end),\\n      y = c(first_bar$x - 0.3, last_bar$x - 0.3),\\n      yend = c(subtotal_row$x + 0.3, subtotal_row$x + 0.3)\\n    )\\n  }))\\n\\n  df_results &lt;- df %&gt;% filter(type == \\\&quot;result\\\&quot;)\\n\\n  # The logic here follows similar logic to the sub-total bars described above\\n  # the slight difference is that since a result is always from zero\\n  # only one connecting line is needed - it connects the top of the previous bar\\n  # (subtotal or otherwise) with the current result bar\\n  df_result_connectors &lt;- bind_rows(lapply(seq_len(nrow(df_results)), function(i) {\\n    result_row &lt;- df_results[i, ]\\n    if (result_row$x == 1) return(NULL)\\n\\n    prev_row &lt;- df %&gt;% filter(x == result_row$x - 1)\\n    if (nrow(prev_row) == 0) return(NULL)\\n\\n    tibble(\\n      x = prev_row$end,\\n      xend = result_row$end,\\n      y = prev_row$x - 0.3,\\n      yend = result_row$x + 0.3\\n    )\\n  }))\\n\\n  # This places all the coordinates of the three types of connecting lines\\n  # into a single tibble so they can all be drawn at once.\\n  df_connectors &lt;- bind_rows(df_lines, df_sub_connectors, df_result_connectors)\\n\\n  ggplot(df %&gt;% filter(type != \\\&quot;divider\\\&quot;)) +\\n    # draw the bars\\n    geom_rect(aes(ymin = x - 0.3, ymax = x + 0.3, xmin = start, xmax = end, fill = fill),\\n              color = NA) +\\n    # draw the connecting lines\\n    geom_segment(\\n      data = df_connectors,\\n      aes(x = x, xend = xend, y = y, yend = yend),\\n      color = \\\&quot;gray70\\\&quot;,\\n      linewidth = 0.2,\\n      inherit.aes = FALSE\\n    ) +\\n    # draw the bar labels\\n    geom_segment(data = df_labels,\\n                 aes(x = label_x, y = x, xend = label_x, yend = x),\\n                 color = \\\&quot;red\\\&quot;, linewidth = 0.2) +\\n    # draw the bar labels\\n    geom_text(data = df_labels,\\n              aes(x = label_x, y = x, label = label, hjust = hjust, fontface = ifelse(bold, \\\&quot;bold\\\&quot;, \\\&quot;plain\\\&quot;)),\\n              size = 3) +\\n    # draw the dividing lines\\n    geom_segment(\\n      data = tibble(y = divider_ys),\\n      aes(x = -Inf, xend = Inf, y = y, yend = y),\\n      linewidth = 0.2,\\n      color = \\\&quot;black\\\&quot;,\\n      inherit.aes = FALSE\\n    ) +\\n    # draw a vertical line at x=0\\n    geom_vline(xintercept = 0, color = \\\&quot;black\\\&quot;, linewidth = 0.2) +\\n    # ensure that the bars are all plotted on the y-axis\\n    # this has the effect of rotating the bar plot from vertical to horizontal bars\\n    scale_y_reverse(\\n      breaks = df$x[df$type != \\\&quot;divider\\\&quot;],\\n      labels = function(labs) {\\n        idx &lt;- match(labs, df$x)\\n        mapply(function(text, bold) {\\n          if (isTRUE(bold)) parse(text = paste0(\\\&quot;bold('\\\&quot;, text, \\\&quot;')\\\&quot;))\\n          else text\\n        }, df$`Line.Item`[idx], df$bold[idx])\\n      }\\n    ) +\\n    coord_cartesian(clip = \\\&quot;off\\\&quot;) +\\n    # scale_x_continuous(expand = expansion(mult = c(0, 0)), limits = c(0, x_max)) +\\n    scale_fill_identity() +\\n    labs(\\n      title = title,\\n      x = NULL,\\n      y = NULL\\n    ) +\\n    theme_minimal(base_size = 11) +\\n    theme(\\n      panel.grid = element_blank(),\\n      plot.title = element_text(hjust = 0.5, face = \\\&quot;bold\\\&quot;)\\n    )\\n}\\n\\nplot_ibcs_variance &lt;- function(\\n    df_raw,\\n    title = \\\&quot;Var.\\\&quot;,\\n    from_col = \\\&quot;Value1\\\&quot;,\\n    to_col = \\\&quot;Value2\\\&quot;,\\n    label_col = \\\&quot;Line.Item\\\&quot;,\\n    var_type = \\\&quot;abs\\\&quot;\\n) {\\n\\n  # Rename user-specified columns to fixed internal names\\n  df_raw &lt;- df_raw %&gt;%\\n    rename(\\n      Value1 = all_of(from_col),\\n      Value2 = all_of(to_col),\\n      `Line.Item` = all_of(label_col)\\n    )\\n\\n  cols &lt;- c(\\\&quot;position\\\&quot;, \\\&quot;type\\\&quot;, \\\&quot;bold\\\&quot;, \\\&quot;subtotal_group\\\&quot;, \\\&quot;Line.Item\\\&quot;, \\\&quot;invert\\\&quot;, \\\&quot;Value1\\\&quot;, \\\&quot;Value2\\\&quot;)\\n  df_raw &lt;- df_raw %&gt;% select(all_of(cols))\\n\\n  # Flag the rows that will be for plotting bars\\n  df &lt;- df_raw %&gt;% mutate(is_plot_row = type != \\\&quot;divider\\\&quot;)\\n\\n  # Assign vertical positions only to non-divider rows\\n  df$x[df$type != \\\&quot;divider\\\&quot;] &lt;- seq_len(sum(df$type != \\\&quot;divider\\\&quot;))\\n\\n  # Compute start\/end for all types\\n  # anchor is always zero for a variance chart, on all bar types (bar, subtotal and result)\\n  anchor &lt;- 0\\n  df &lt;- df %&gt;%\\n    mutate(\\n      end = if (var_type == \\\&quot;abs\\\&quot;) {\\n        (Value2 - Value1) * if_else(invert, -1, 1)\\n      } else {\\n        (100 * (Value2 - Value1) \/ Value1)\\n      },\\n      start = anchor\\n    )\\n\\n\\n\\n  for (i in seq_len(nrow(df))) {\\n    row_type &lt;- df$type[i]\\n    invert &lt;- df$invert[i]\\n    if (row_type == \\\&quot;subtotal\\\&quot;) {\\n      group_id &lt;- df$subtotal_group[i]\\n\\n      bar_rows &lt;- which(df$subtotal_group == group_id &amp; df$type == \\\&quot;bar\\\&quot;)\\n      if (length(bar_rows) &gt; 0) {\\n        val1 &lt;- sum(df$Value1[bar_rows], na.rm = TRUE)\\n        val2 &lt;- sum(df$Value2[bar_rows], na.rm = TRUE)\\n        df$Value1[i] &lt;- val1\\n        df$Value2[i] &lt;- val2\\n        df$end[i] = if (var_type == \\\&quot;abs\\\&quot;) {\\n          (val2 - val1) * if_else(invert, -1, 1)\\n        } else {\\n          (100 * (val2 - val1) \/ val1)\\n        }\\n      }\\n\\n    } else if (row_type == \\\&quot;result\\\&quot;) {\\n      # Get all rows above this one that are bars\\n      bar_rows_above &lt;- df[1:(i - 1), ] %&gt;% filter(type == \\\&quot;bar\\\&quot;)\\n      total_var &lt;- if (var_type == \\\&quot;abs\\\&quot;) {\\n        sum(bar_rows_above$end * if_else(bar_rows_above$invert, -1, 1), na.rm = TRUE)\\n      } else {\\n        val1 &lt;- sum(bar_rows_above$Value1)\\n        (100 * (sum(bar_rows_above$Value2) - val1) \/ val1) * if_else(invert, -1, 1)\\n      }\\n\\n      df$start[i] &lt;- anchor\\n      df$end[i] &lt;- total_var\\n\\n    }\\n  }\\n\\n  bad_color &lt;- \\\&quot;indianred3\\\&quot;   # softer than \\\&quot;red\\\&quot;\\n  good_color &lt;- \\\&quot;chartreuse3\\\&quot;  # softer than \\\&quot;green\\\&quot;\\n\\n  # Assign fill colors to drawn bars\\n  # Positive bars are gray with 70% transparency\\n  # Negative bars are gray with 30% transparency\\n  df &lt;- df %&gt;%\\n    mutate(\\n      fill = case_when(\\n        type == \\\&quot;divider\\\&quot; ~ NA_character_,\\n        is.na(end) ~ NA_character_,\\n        invert &amp; end &gt;= 0 ~ bad_color,       # Expense ↑ → bad\\n        invert &amp; end &lt; 0 ~ good_color,      # Expense ↓ → good\\n        !invert &amp; end &gt;= 0 ~ good_color,    # Income ↑ → good\\n        TRUE ~ bad_color                     # Income ↓ → bad\\n      )\\n    )\\n\\n\\n  # Format the bar labels\\n  # Currently zero decimal places\\n  # Negative bars have their labels to the left of the bar\\n  # Positive bars have their labels to the right of the bar\\n  # Negative bars don't use the minus symbol\\n  df_labels &lt;- df %&gt;%\\n    filter(type != \\\&quot;divider\\\&quot;) %&gt;%\\n    mutate(\\n      label = formatC(round(end, 0), format = \\\&quot;f\\\&quot;, digits = 0, flag = \\\&quot;+\\\&quot;),\\n      label_x = if_else(end &gt;= 0, end + 5, end - 5),\\n      hjust = if_else(end &gt;= 0, 0, 1)\\n    )\\n\\n  # this will be used to extend the x-axis to allow space for bar labels\\n  # x_max &lt;- max(df_labels$label_x, na.rm = TRUE) + 100  # 10 is padding\\n\\n  # divider_ys is a numeric vector of vertical positions\\n  # at which horizontal lines will be drawn to separate\\n  # bars from one another at the user's discretion\\n  divider_ys &lt;- df %&gt;%\\n    mutate(idx = row_number()) %&gt;%\\n    filter(type == \\\&quot;divider\\\&quot;) %&gt;%\\n    mutate(\\n      prev_x = df$x[idx - 1],\\n      next_x = df$x[idx + 1],\\n      y = (prev_x + next_x) \/ 2\\n    ) %&gt;%\\n    pull(y) # extracts this tibble column to a vector\\n\\n  ggplot(df %&gt;% filter(type != \\\&quot;divider\\\&quot;)) +\\n    # draw the bars\\n    geom_rect(aes(ymin = x - 0.3, ymax = x + 0.3, xmin = start, xmax = end, fill = fill),\\n              color = NA) +\\n    # draw the bar labels\\n    geom_text(data = df_labels,\\n              aes(x = label_x, y = x, label = label, hjust = hjust, fontface = ifelse(bold, \\\&quot;bold\\\&quot;, \\\&quot;plain\\\&quot;)),\\n              size = 3) +\\n    # draw the dividing lines\\n    geom_segment(\\n      data = tibble(y = divider_ys),\\n      aes(x = -Inf, xend = Inf, y = y, yend = y),\\n      linewidth = 0.2,\\n      color = \\\&quot;black\\\&quot;,\\n      inherit.aes = FALSE\\n    ) +\\n    # draw a vertical line at x=0\\n    geom_vline(xintercept = 0, color = \\\&quot;black\\\&quot;, linewidth = 0.2) +\\n    # ensure that the bars are all plotted on the y-axis\\n    # this has the effect of rotating the bar plot from vertical to horizontal bars\\n    scale_y_reverse(\\n      breaks = df$x[df$type != \\\&quot;divider\\\&quot;],\\n      labels = function(labs) {\\n        idx &lt;- match(labs, df$x)\\n        mapply(function(text, bold) {\\n          if (isTRUE(bold)) parse(text = paste0(\\\&quot;bold('\\\&quot;, text, \\\&quot;')\\\&quot;))\\n          else text\\n        }, df$`Line.Item`[idx], df$bold[idx])\\n      }\\n    ) +\\n    coord_cartesian(clip = \\\&quot;off\\\&quot;) +\\n    # scale_x_continuous(expand = expansion(mult = c(0, 0)), limits = c(0, x_max)) +\\n    scale_fill_identity() +\\n    labs(\\n      title = title,\\n      x = NULL,\\n      y = NULL\\n    ) +\\n    theme_minimal(base_size = 11) +\\n    theme(\\n      panel.grid = element_blank(),\\n      plot.title = element_text(hjust = 0.5, face = \\\&quot;bold\\\&quot;)\\n    )\\n}\\n\\n## Pre-built utility functions\\n\\n# Convert to tibble or data.frame\\nto_dataframe &lt;- function(x, as_tibble=TRUE) {\\n  if (inherits(x, \\\&quot;data.frame\\\&quot;)) {\\n    return(x)\\n  }\\n  if (!is_list_of_lists(x)) {\\n    stop(\\\&quot;Expected list of lists\\\&quot;)\\n  }\\n\\n  # Get column names from first row if available\\n  if (length(x) &gt; 1) {\\n    col_names &lt;- x[[1]]\\n    data_rows &lt;- x[-1]\\n  } else {\\n    data_rows &lt;- x\\n    col_names &lt;- paste0(\\\&quot;V\\\&quot;, seq_len(length(x[[1]])))\\n  }\\n  # Convert to column-wise list preserving data types\\n  cols &lt;- to_colwise_list(data_rows)\\n  names(cols) &lt;- col_names\\n\\n  # Create data frame preserving column types\\n  df &lt;- as.data.frame(cols, stringsAsFactors = FALSE)\\n\\n  if (as_tibble) {\\n    if (!requireNamespace(\\\&quot;dplyr\\\&quot;, quietly = TRUE)) {\\n      warning(\\\&quot;Package 'dplyr' needed for tibble conversion\\\&quot;)\\n    } else {\\n      return(dplyr::as_tibble(df))\\n    }\\n  }\\n  return(df)\\n}\\n\\n\\n# Convert to matrix\\nto_matrix &lt;- function(x) {\\n  if (is.matrix(x)) {\\n    return(x)\\n  }\\n  if (!is_list_of_lists(x)) {\\n    stop(\\\&quot;Expected list of lists\\\&quot;)\\n  }\\n  return(do.call(rbind, lapply(x, unlist)))\\n}\\n\\n# Convert to colwise list of vectors\\n# to_colwise_list &lt;- function(x) {\\n#   if (!is_list_of_lists(x)) {\\n#     stop(\\\&quot;Expected list of lists\\\&quot;)\\n#   }\\n\\n#   ncols &lt;- length(x[[1]])\\n#   print(ncols)\\n#   print(seq_len(ncols))\\n#   lapply(seq_len(ncols), function(j) {\\n#     print(j)\\n#     do.call(c, lapply(seq_along(x), function(i) x[[i]][[j]]))\\n#   })\\n# }\\n\\nto_colwise_list &lt;- function(x) {\\n  if (!is_list_of_lists(x)) {\\n    stop(\\\&quot;Expected list of lists\\\&quot;)\\n  }\\n\\n  ncols &lt;- length(x[[1]])\\n  lapply(seq_len(ncols), function(j) {\\n    do.call(c, lapply(seq_along(x), function(i) {\\n      val &lt;- x[[i]][[j]]\\n      if (is.null(val)) NA else val\\n    }))\\n  })\\n}\\n\\n\\n\\nis_list_of_lists &lt;- function(x) {\\n  is.list(x) &amp;&amp; length(x) &gt; 0 &amp;&amp; is.list(x[[1]])\\n}\\n\\n\&quot;}&quot;"/>
+    <we:property name="rworkerConfig" value="&quot;{\&quot;webrVersion\&quot;:\&quot;0.4.2\&quot;,\&quot;webrPackages\&quot;:[\&quot;jsonlite\&quot;,\&quot;sloop\&quot;,\&quot;tidyverse\&quot;,\&quot;patchwork\&quot;],\&quot;initCode\&quot;:\&quot;## Add imports\\nlibrary(tidyverse)\\nlibrary(patchwork)\\n\\n## Configuration\\noptions(warnPartialMatchDollar = TRUE)\\n\\n## Define functions\\nplot_ibcs_waterfall &lt;- function(\\n  df_raw,\\n  title = \\\&quot;Waterfall Chart\\\&quot;,\\n  value_col = \\\&quot;Value\\\&quot;,\\n  label_col = \\\&quot;Line.Item\\\&quot;\\n) {\\n\\n  # Rename user-specified columns to fixed internal names\\n  df_raw &lt;- df_raw %&gt;%\\n    rename(\\n      Value = all_of(value_col),\\n      `Line.Item` = all_of(label_col)\\n    )\\n\\n  cols &lt;- c(\\\&quot;position\\\&quot;, \\\&quot;type\\\&quot;, \\\&quot;bold\\\&quot;, \\\&quot;subtotal_group\\\&quot;, \\\&quot;Line.Item\\\&quot;, \\\&quot;Value\\\&quot;)\\n  df_raw &lt;- df_raw %&gt;% select(all_of(cols))\\n\\n  # Flag the rows that will be for plotting bars\\n  df &lt;- df_raw %&gt;% mutate(is_plot_row = type != \\\&quot;divider\\\&quot;)\\n\\n  # Assign vertical positions only to non-divider rows\\n  df$x[df$type != \\\&quot;divider\\\&quot;] &lt;- seq_len(sum(df$type != \\\&quot;divider\\\&quot;))\\n\\n  # Compute start\/end for all types\\n  anchor &lt;- 0\\n  for (i in seq_len(nrow(df))) {\\n    row_type &lt;- df$type[i]\\n\\n    if (row_type == \\\&quot;bar\\\&quot;) {\\n      df$start[i] &lt;- anchor\\n      df$end[i] &lt;- anchor + df$Value[i]\\n      anchor &lt;- df$end[i]\\n\\n    } else if (row_type == \\\&quot;subtotal\\\&quot;) {\\n      group_id &lt;- df$subtotal_group[i]\\n      bar_rows &lt;- which(df$subtotal_group == group_id &amp; df$type == \\\&quot;bar\\\&quot;)\\n      if (length(bar_rows) &gt; 0) {\\n        subtotal_value &lt;- sum(df$Value[bar_rows], na.rm = TRUE)\\n        df$Value[i] &lt;- subtotal_value\\n        group_start &lt;- df$start[bar_rows[1]]\\n        df$start[i] &lt;- group_start\\n        df$end[i] &lt;- group_start + subtotal_value\\n        anchor &lt;- df$end[i]\\n      }\\n\\n    } else if (row_type == \\\&quot;result\\\&quot;) {\\n      df$start[i] &lt;- 0\\n      df$end[i] &lt;- anchor\\n      df$Value[i] &lt;- anchor\\n      anchor &lt;- df$end[i]\\n    }\\n  }\\n\\n  # calculate the coordinates for non-subtotal and non-result connecting lines\\n  df_lines &lt;- df %&gt;%\\n    filter(type != \\\&quot;divider\\\&quot;) %&gt;%\\n    arrange(x) %&gt;%\\n    mutate(\\n      x_next = lead(x),\\n      xend = lead(start)\\n    ) %&gt;%\\n    filter(!is.na(x_next)) %&gt;%\\n    transmute(\\n      y = x - 0.3, # from the vertical top of the current bar\\n      yend = x_next + 0.3, # to the vertical bottom of the next bar\\n      x = xend,\\n      xend\\n    )\\n\\n  # Assign fill colors to drawn bars\\n  # Positive bars are gray with 70% transparency\\n  # Negative bars are gray with 30% transparency\\n  df &lt;- df %&gt;%\\n    mutate(\\n      fill = case_when(\\n        type == \\\&quot;divider\\\&quot; ~ NA_character_,\\n        Value &gt;= 0 ~ \\\&quot;gray70\\\&quot;,\\n        TRUE ~ \\\&quot;gray30\\\&quot;\\n      )\\n    )\\n\\n  # Format the bar labels\\n  # Currently zero decimal places\\n  # Negative bars have their labels to the left of the bar\\n  # Positive bars have their labels to the right of the bar\\n  # Negative bars don't use the minus symbol\\n  df_labels &lt;- df %&gt;%\\n    filter(type != \\\&quot;divider\\\&quot;) %&gt;%\\n    mutate(\\n      label = format(round(abs(Value), 0), nsmall = 0),\\n      label_x = if_else(Value &gt;= 0, end + 5, end - 5),\\n      hjust = if_else(Value &gt;= 0, 0, 1)\\n    )\\n\\n  # this will be used to extend the x-axis to allow space for bar labels\\n  # x_max &lt;- max(df_labels$label_x, na.rm = TRUE) + 100  # 10 is padding\\n\\n  # divider_ys is a numeric vector of vertical positions\\n  # at which horizontal lines will be drawn to separate\\n  # bars from one another at the user's discretion\\n  divider_ys &lt;- df %&gt;%\\n    mutate(idx = row_number()) %&gt;%\\n    filter(type == \\\&quot;divider\\\&quot;) %&gt;%\\n    mutate(\\n      prev_x = df$x[idx - 1],\\n      next_x = df$x[idx + 1],\\n      y = (prev_x + next_x) \/ 2\\n    ) %&gt;%\\n    pull(y) # extracts this tibble column to a vector\\n\\n  df_subtotals &lt;- df %&gt;% filter(type == \\\&quot;subtotal\\\&quot;)\\n\\n  # Apply a function over a list of integers from 1 to count of sub total rows\\n  df_sub_connectors &lt;- bind_rows(lapply(seq_len(nrow(df_subtotals)), function(i) {\\n    # Get the current row\\n    subtotal_row &lt;- df_subtotals[i, ]\\n    # Get the current group id\\n    group_id &lt;- subtotal_row$subtotal_group\\n    # Get the bar rows from df whose group id matches the current subtotal row\\n    bar_rows &lt;- df %&gt;% filter(type == \\\&quot;bar\\\&quot;, subtotal_group == group_id)\\n\\n    # If there are no such bars, then this subtotal is invalid (user incorrectly defined)\\n    if (nrow(bar_rows) &lt; 1) return(NULL)\\n\\n    # There are two lines which visually connect a subtotal with its components:\\n    # 1) A line from the bottom (i.e. left) of the first bar in the group\\n    # to the bottom (i.e. left) of the sub-total bar\\n    # 2) A line from the top (i.e. right) of the last bar in the group\\n    # to the top (i.e. right) of the sub-total bar\\n    first_bar &lt;- bar_rows[1, ]\\n    last_bar &lt;- bar_rows[nrow(bar_rows), ]\\n\\n    # Each sub-total produces two rows representing the lines connecting the \\n    # bars with their associated sub-total bar\\n    tibble(\\n      x = c(first_bar$start, last_bar$end),\\n      xend = c(first_bar$start, last_bar$end),\\n      y = c(first_bar$x - 0.3, last_bar$x - 0.3),\\n      yend = c(subtotal_row$x + 0.3, subtotal_row$x + 0.3)\\n    )\\n  }))\\n\\n  df_results &lt;- df %&gt;% filter(type == \\\&quot;result\\\&quot;)\\n\\n  # The logic here follows similar logic to the sub-total bars described above\\n  # the slight difference is that since a result is always from zero\\n  # only one connecting line is needed - it connects the top of the previous bar\\n  # (subtotal or otherwise) with the current result bar\\n  df_result_connectors &lt;- bind_rows(lapply(seq_len(nrow(df_results)), function(i) {\\n    result_row &lt;- df_results[i, ]\\n    if (result_row$x == 1) return(NULL)\\n\\n    prev_row &lt;- df %&gt;% filter(x == result_row$x - 1)\\n    if (nrow(prev_row) == 0) return(NULL)\\n\\n    tibble(\\n      x = prev_row$end,\\n      xend = result_row$end,\\n      y = prev_row$x - 0.3,\\n      yend = result_row$x + 0.3\\n    )\\n  }))\\n\\n  # This places all the coordinates of the three types of connecting lines\\n  # into a single tibble so they can all be drawn at once.\\n  df_connectors &lt;- bind_rows(df_lines, df_sub_connectors, df_result_connectors)\\n\\n  ggplot(df %&gt;% filter(type != \\\&quot;divider\\\&quot;)) +\\n    # draw the bars\\n    geom_rect(aes(ymin = x - 0.3, ymax = x + 0.3, xmin = start, xmax = end, fill = fill),\\n              color = NA) +\\n    # draw the connecting lines\\n    geom_segment(\\n      data = df_connectors,\\n      aes(x = x, xend = xend, y = y, yend = yend),\\n      color = \\\&quot;gray70\\\&quot;,\\n      linewidth = 0.2,\\n      inherit.aes = FALSE\\n    ) +\\n    # draw the bar labels\\n    geom_segment(data = df_labels,\\n                 aes(x = label_x, y = x, xend = label_x, yend = x),\\n                 color = \\\&quot;red\\\&quot;, linewidth = 0.2) +\\n    # draw the bar labels\\n    geom_text(data = df_labels,\\n              aes(x = label_x, y = x, label = label, hjust = hjust, fontface = ifelse(bold, \\\&quot;bold\\\&quot;, \\\&quot;plain\\\&quot;)),\\n              size = 3) +\\n    # draw the dividing lines\\n    geom_segment(\\n      data = tibble(y = divider_ys),\\n      aes(x = -Inf, xend = Inf, y = y, yend = y),\\n      linewidth = 0.2,\\n      color = \\\&quot;black\\\&quot;,\\n      inherit.aes = FALSE\\n    ) +\\n    # draw a vertical line at x=0\\n    geom_vline(xintercept = 0, color = \\\&quot;black\\\&quot;, linewidth = 0.2) +\\n    # ensure that the bars are all plotted on the y-axis\\n    # this has the effect of rotating the bar plot from vertical to horizontal bars\\n    scale_y_reverse(\\n      breaks = df$x[df$type != \\\&quot;divider\\\&quot;],\\n      labels = function(labs) {\\n        idx &lt;- match(labs, df$x)\\n        mapply(function(text, bold) {\\n          if (isTRUE(bold)) parse(text = paste0(\\\&quot;bold('\\\&quot;, text, \\\&quot;')\\\&quot;))\\n          else text\\n        }, df$`Line.Item`[idx], df$bold[idx])\\n      }\\n    ) +\\n    coord_cartesian(clip = \\\&quot;off\\\&quot;) +\\n    # scale_x_continuous(expand = expansion(mult = c(0, 0)), limits = c(0, x_max)) +\\n    scale_fill_identity() +\\n    labs(\\n      title = title,\\n      size = 15,\\n      x = NULL,\\n      y = NULL\\n    ) +\\n    theme_minimal(base_size = 11) +\\n    theme(\\n      panel.grid = element_blank(),\\n      plot.title.position = 'panel'\\n    )\\n}\\n\\nplot_ibcs_variance &lt;- function(\\n    df_raw,\\n    title = \\\&quot;Var.\\\&quot;,\\n    from_col = \\\&quot;Value1\\\&quot;,\\n    to_col = \\\&quot;Value2\\\&quot;,\\n    label_col = \\\&quot;Line.Item\\\&quot;,\\n    var_type = \\\&quot;abs\\\&quot;\\n) {\\n\\n  # Rename user-specified columns to fixed internal names\\n  df_raw &lt;- df_raw %&gt;%\\n    rename(\\n      Value1 = all_of(from_col),\\n      Value2 = all_of(to_col),\\n      `Line.Item` = all_of(label_col)\\n    )\\n\\n  cols &lt;- c(\\\&quot;position\\\&quot;, \\\&quot;type\\\&quot;, \\\&quot;bold\\\&quot;, \\\&quot;subtotal_group\\\&quot;, \\\&quot;Line.Item\\\&quot;, \\\&quot;invert\\\&quot;, \\\&quot;Value1\\\&quot;, \\\&quot;Value2\\\&quot;)\\n  df_raw &lt;- df_raw %&gt;% select(all_of(cols))\\n\\n  # Flag the rows that will be for plotting bars\\n  df &lt;- df_raw %&gt;% mutate(is_plot_row = type != \\\&quot;divider\\\&quot;)\\n\\n  # Assign vertical positions only to non-divider rows\\n  df$x[df$type != \\\&quot;divider\\\&quot;] &lt;- seq_len(sum(df$type != \\\&quot;divider\\\&quot;))\\n\\n  # Compute start\/end for all types\\n  # anchor is always zero for a variance chart, on all bar types (bar, subtotal and result)\\n  anchor &lt;- 0\\n  df &lt;- df %&gt;%\\n    mutate(\\n      end = if (var_type == \\\&quot;abs\\\&quot;) {\\n        (Value2 - Value1) * if_else(invert, -1, 1)\\n      } else {\\n        (100 * (Value2 - Value1) \/ Value1)\\n      },\\n      start = anchor\\n    )\\n\\n\\n\\n  for (i in seq_len(nrow(df))) {\\n    row_type &lt;- df$type[i]\\n    invert &lt;- df$invert[i]\\n    if (row_type == \\\&quot;subtotal\\\&quot;) {\\n      group_id &lt;- df$subtotal_group[i]\\n\\n      bar_rows &lt;- which(df$subtotal_group == group_id &amp; df$type == \\\&quot;bar\\\&quot;)\\n      if (length(bar_rows) &gt; 0) {\\n        val1 &lt;- sum(df$Value1[bar_rows], na.rm = TRUE)\\n        val2 &lt;- sum(df$Value2[bar_rows], na.rm = TRUE)\\n        df$Value1[i] &lt;- val1\\n        df$Value2[i] &lt;- val2\\n        df$end[i] = if (var_type == \\\&quot;abs\\\&quot;) {\\n          (val2 - val1) * if_else(invert, -1, 1)\\n        } else {\\n          (100 * (val2 - val1) \/ val1)\\n        }\\n      }\\n\\n    } else if (row_type == \\\&quot;result\\\&quot;) {\\n      # Get all rows above this one that are bars\\n      bar_rows_above &lt;- df[1:(i - 1), ] %&gt;% filter(type == \\\&quot;bar\\\&quot;)\\n      total_var &lt;- if (var_type == \\\&quot;abs\\\&quot;) {\\n        sum(bar_rows_above$end * if_else(bar_rows_above$invert, -1, 1), na.rm = TRUE)\\n      } else {\\n        val1 &lt;- sum(bar_rows_above$Value1)\\n        (100 * (sum(bar_rows_above$Value2) - val1) \/ val1) * if_else(invert, -1, 1)\\n      }\\n\\n      df$start[i] &lt;- anchor\\n      df$end[i] &lt;- total_var\\n\\n    }\\n  }\\n\\n  bad_color &lt;- \\\&quot;indianred3\\\&quot;   # softer than \\\&quot;red\\\&quot;\\n  good_color &lt;- \\\&quot;chartreuse3\\\&quot;  # softer than \\\&quot;green\\\&quot;\\n\\n  # Assign fill colors to drawn bars\\n  # Positive bars are gray with 70% transparency\\n  # Negative bars are gray with 30% transparency\\n  df &lt;- df %&gt;%\\n    mutate(\\n      fill = case_when(\\n        type == \\\&quot;divider\\\&quot; ~ NA_character_,\\n        is.na(end) ~ NA_character_,\\n        invert &amp; end &gt;= 0 ~ bad_color,       # Expense ↑ → bad\\n        invert &amp; end &lt; 0 ~ good_color,      # Expense ↓ → good\\n        !invert &amp; end &gt;= 0 ~ good_color,    # Income ↑ → good\\n        TRUE ~ bad_color                     # Income ↓ → bad\\n      )\\n    )\\n\\n\\n  # Format the bar labels\\n  # Currently zero decimal places\\n  # Negative bars have their labels to the left of the bar\\n  # Positive bars have their labels to the right of the bar\\n  # Negative bars don't use the minus symbol\\n  df_labels &lt;- df %&gt;%\\n    filter(type != \\\&quot;divider\\\&quot;) %&gt;%\\n    mutate(\\n      label = formatC(round(end, 0), format = \\\&quot;f\\\&quot;, digits = 0, flag = \\\&quot;+\\\&quot;),\\n      label_x = if_else(end &gt;= 0, end + 5, end - 5),\\n      hjust = if_else(end &gt;= 0, 0, 1)\\n    )\\n\\n  # this will be used to extend the x-axis to allow space for bar labels\\n  # x_max &lt;- max(df_labels$label_x, na.rm = TRUE) + 100  # 10 is padding\\n\\n  # divider_ys is a numeric vector of vertical positions\\n  # at which horizontal lines will be drawn to separate\\n  # bars from one another at the user's discretion\\n  divider_ys &lt;- df %&gt;%\\n    mutate(idx = row_number()) %&gt;%\\n    filter(type == \\\&quot;divider\\\&quot;) %&gt;%\\n    mutate(\\n      prev_x = df$x[idx - 1],\\n      next_x = df$x[idx + 1],\\n      y = (prev_x + next_x) \/ 2\\n    ) %&gt;%\\n    pull(y) # extracts this tibble column to a vector\\n\\n  ggplot(df %&gt;% filter(type != \\\&quot;divider\\\&quot;)) +\\n    # draw the bars\\n    geom_rect(aes(ymin = x - 0.3, ymax = x + 0.3, xmin = start, xmax = end, fill = fill),\\n              color = NA) +\\n    # draw the bar labels\\n    geom_text(data = df_labels,\\n              aes(x = label_x, y = x, label = label, hjust = hjust, fontface = ifelse(bold, \\\&quot;bold\\\&quot;, \\\&quot;plain\\\&quot;)),\\n              size = 3) +\\n    # draw the dividing lines\\n    geom_segment(\\n      data = tibble(y = divider_ys),\\n      aes(x = -Inf, xend = Inf, y = y, yend = y),\\n      linewidth = 0.2,\\n      color = \\\&quot;black\\\&quot;,\\n      inherit.aes = FALSE\\n    ) +\\n    # draw a vertical line at x=0\\n    geom_vline(xintercept = 0, color = \\\&quot;black\\\&quot;, linewidth = 0.2) +\\n    # ensure that the bars are all plotted on the y-axis\\n    # this has the effect of rotating the bar plot from vertical to horizontal bars\\n    scale_y_reverse(\\n      breaks = df$x[df$type != \\\&quot;divider\\\&quot;],\\n      labels = function(labs) {\\n        idx &lt;- match(labs, df$x)\\n        mapply(function(text, bold) {\\n          if (isTRUE(bold)) parse(text = paste0(\\\&quot;bold('\\\&quot;, text, \\\&quot;')\\\&quot;))\\n          else text\\n        }, df$`Line.Item`[idx], df$bold[idx])\\n      }\\n    ) +\\n    coord_cartesian(clip = \\\&quot;off\\\&quot;) +\\n    # scale_x_continuous(expand = expansion(mult = c(0, 0)), limits = c(0, x_max)) +\\n    scale_fill_identity() +\\n    labs(\\n      title = title,\\n      x = NULL,\\n      y = NULL\\n    ) +\\n    theme_minimal(base_size = 11) +\\n    theme(\\n      panel.grid = element_blank(),\\n      plot.title.position = 'panel'\\n    )\\n}\\n\\n## Pre-built utility functions\\n\\n# Convert to tibble or data.frame\\nto_dataframe &lt;- function(x, as_tibble=TRUE) {\\n  if (inherits(x, \\\&quot;data.frame\\\&quot;)) {\\n    return(x)\\n  }\\n  if (!is_list_of_lists(x)) {\\n    stop(\\\&quot;Expected list of lists\\\&quot;)\\n  }\\n\\n  # Get column names from first row if available\\n  if (length(x) &gt; 1) {\\n    col_names &lt;- x[[1]]\\n    data_rows &lt;- x[-1]\\n  } else {\\n    data_rows &lt;- x\\n    col_names &lt;- paste0(\\\&quot;V\\\&quot;, seq_len(length(x[[1]])))\\n  }\\n  # Convert to column-wise list preserving data types\\n  cols &lt;- to_colwise_list(data_rows)\\n  names(cols) &lt;- col_names\\n\\n  # Create data frame preserving column types\\n  df &lt;- as.data.frame(cols, stringsAsFactors = FALSE)\\n\\n  if (as_tibble) {\\n    if (!requireNamespace(\\\&quot;dplyr\\\&quot;, quietly = TRUE)) {\\n      warning(\\\&quot;Package 'dplyr' needed for tibble conversion\\\&quot;)\\n    } else {\\n      return(dplyr::as_tibble(df))\\n    }\\n  }\\n  return(df)\\n}\\n\\n\\n# Convert to matrix\\nto_matrix &lt;- function(x) {\\n  if (is.matrix(x)) {\\n    return(x)\\n  }\\n  if (!is_list_of_lists(x)) {\\n    stop(\\\&quot;Expected list of lists\\\&quot;)\\n  }\\n  return(do.call(rbind, lapply(x, unlist)))\\n}\\n\\n# Convert to colwise list of vectors\\n# to_colwise_list &lt;- function(x) {\\n#   if (!is_list_of_lists(x)) {\\n#     stop(\\\&quot;Expected list of lists\\\&quot;)\\n#   }\\n\\n#   ncols &lt;- length(x[[1]])\\n#   print(ncols)\\n#   print(seq_len(ncols))\\n#   lapply(seq_len(ncols), function(j) {\\n#     print(j)\\n#     do.call(c, lapply(seq_along(x), function(i) x[[i]][[j]]))\\n#   })\\n# }\\n\\nto_colwise_list &lt;- function(x) {\\n  if (!is_list_of_lists(x)) {\\n    stop(\\\&quot;Expected list of lists\\\&quot;)\\n  }\\n\\n  ncols &lt;- length(x[[1]])\\n  lapply(seq_len(ncols), function(j) {\\n    do.call(c, lapply(seq_along(x), function(i) {\\n      val &lt;- x[[i]][[j]]\\n      if (is.null(val)) NA else val\\n    }))\\n  })\\n}\\n\\n\\n\\nis_list_of_lists &lt;- function(x) {\\n  is.list(x) &amp;&amp; length(x) &gt; 0 &amp;&amp; is.list(x[[1]])\\n}\\n\\n\&quot;}&quot;"/>
   </we:properties>
   <we:bindings>
     <we:binding id="pyscript_a970bdb0-b52c-4e67-b5b3-96823e097d1f" type="matrix" appref="{E7B16A11-FC0F-40D7-8C7F-63DFEB259E62}"/>
@@ -794,7 +794,7 @@
   <dimension ref="B1:I34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -896,37 +896,47 @@
       <c r="C6" t="e" cm="1" vm="5">
         <f t="array" ref="C6">_xldudf_ANACONDA_CODE("r", "### Do Not Edit this formula directly. Use Anaconda Code to modify.
 data &lt;- to_dataframe(REF($P3$))
+theming &lt;- theme(
+  axis.text.y = element_blank(), 
+  axis.text.x = element_blank(),
+  plot.title.position = 'plot'
+  )
 py &lt;- plot_ibcs_waterfall(
-  df_raw = data,
+  df_r"&amp;"aw = data,
   title = ""PY"",
   value_col = ""PY"",
   label_col = ""Line.Item""
 )+ theme(axis.text.x = element_blank())
-c"&amp;"y &lt;- plot_ibcs_waterfall(
+cy &lt;- plot_ibcs_waterfall(
   df_raw = data,
   title = ""Actuals"",
   value_col = ""AC"",
   label_col = ""Line.Item""
-) + theme(axis.text.y = element_blank(), axis.text.x = element_blank())
-var_abs &lt;- plot_ibcs_variance(
+) + theming
+var_a"&amp;"bs &lt;- plot_ibcs_variance(
   df_raw = data,
-  title = ""Var."&amp;""",
+  title = ""Var."",
   from_col = ""PY"",
   to_col = ""AC"",
   label_col = ""Line.Item"",
   var_type = ""abs""
-) + theme(axis.text.y = element_blank(), axis.text.x = element_blank())
+) + theming
 var_pct &lt;- plot_ibcs_variance(
   df_raw = data,
   title = ""%"",
   from_col = ""PY"",
- "&amp;" to_col = ""AC"",
+  "&amp;"to_col = ""AC"",
   label_col = ""Line.Item"",
   var_type = ""pct""
-) + theme(axis.text.y = element_blank(), axis.text.x = element_blank())
+) + theming
 library(patchwork)
 (py | cy | plot_spacer() | var_abs | var_pct | plot_spacer()) + 
-  plot_layout(widths = c(1, 1"&amp;", 0.1, 0.5, 0.5, 0.1))
+  plot_layout(widths = c(1, 1, 0.1, 0.5, 0.5, 0.1)) + 
+  plot_annotation(
+  title = 'Curre"&amp;"nt year actuals vs. previous year',
+  subtitle = 'Variances shown in absolute and relative % terms',
+  caption = 'Produced with plotibcs and patchwork'
+)
 ", 2, dat[#All])</f>
         <v>#VALUE!</v>
       </c>

</xml_diff>